<commit_message>
Original file for classes and subclasses added,
</commit_message>
<xml_diff>
--- a/SmallQuranWords - Test.xlsx
+++ b/SmallQuranWords - Test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\University\4002 - Ahmadi Roshan\Python Codes for Ontology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\University\4002 - Ahmadi Roshan\Python Codes for Ontology\QuranOntology\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="0" windowWidth="16560" windowHeight="6384"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="22104" windowHeight="9972"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,51 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>قرائات و قراء</t>
-  </si>
-  <si>
-    <t>قرائت به روایت</t>
-  </si>
-  <si>
-    <t>فواتح خبری</t>
-  </si>
-  <si>
-    <t>قرائت صحابه</t>
-  </si>
-  <si>
-    <t>قرائت ابن عامر یحصبی</t>
-  </si>
-  <si>
-    <t>قرائت بادیه‌نشینان</t>
-  </si>
-  <si>
-    <t>قرائت سماعی</t>
-  </si>
-  <si>
-    <t>قراء تابعین کوفی</t>
-  </si>
-  <si>
-    <t>قرّای اربعه عشر</t>
-  </si>
-  <si>
-    <t>قرائات اربعه  عشر</t>
-  </si>
-  <si>
-    <t>فواتح سور</t>
-  </si>
-  <si>
-    <t>قانون ترجیح در رای</t>
-  </si>
-  <si>
-    <t>قرّای اهل تالیف</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>ادغام علوم قرآن و معارف قرآن با لحاظ ادغام مشترکات لفظی</t>
-  </si>
-  <si>
-    <t>قاعده عمومیت لفظ یا خصوص سبب</t>
   </si>
 </sst>
 </file>
@@ -431,11 +389,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -448,77 +404,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>